<commit_message>
Added fix to pregnancy condition cards and household assessment form
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/household_assessment.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/household_assessment.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="263">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">malaria_prone</t>
   </si>
   <si>
-    <t xml:space="preserve">../household_assessment/wire_mesh_on_inlets = 'yes' or ../household_assessment/stagnant_water = 'yes' or ../household_assessment/nets_availability = 'no' or ../household_assessment/proper_drainage = 'no' or ../household_assessment/resedual_spraying = 'no' or ../household_assessment/tall_grass = 'yes'</t>
+    <t xml:space="preserve">../household_assessment/wire_mesh_on_inlets = 'no' or ../household_assessment/stagnant_water = 'yes' or ../household_assessment/nets_availability = 'no' or ../household_assessment/proper_drainage = 'no' or ../household_assessment/resedual_spraying = 'no' or ../household_assessment/tall_grass = 'yes'</t>
   </si>
   <si>
     <t xml:space="preserve">referral_follow_up_date</t>
@@ -473,16 +473,13 @@
     <t xml:space="preserve">${place_name} is not prone to malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(${wire_mesh_on_inlets}, ‘yes’) and selected(${nets_availability}, ‘yes’) and selected(${tall_grass}, ‘yes’) and selected(${stagnant_water}, no)</t>
+    <t xml:space="preserve">${malaria_prone} = ‘false’ </t>
   </si>
   <si>
     <t xml:space="preserve">r_prone</t>
   </si>
   <si>
     <t xml:space="preserve">${place_name} is prone to malaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(${wire_mesh_on_inlets}, ‘no’) or selected(${nets_availability}, ‘no’) or selected(${tall_grass}, ‘no’) or selected(${stagnant_water}, ‘yes’)</t>
   </si>
   <si>
     <t xml:space="preserve">h5 center red</t>
@@ -873,7 +870,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -947,6 +944,11 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1110,7 +1112,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1223,39 +1225,55 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1263,27 +1281,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1291,7 +1297,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1375,14 +1381,14 @@
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="I44" activeCellId="0" sqref="I44"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="K52" activeCellId="0" sqref="K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.29"/>
@@ -3516,7 +3522,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="23" t="s">
         <v>81</v>
       </c>
@@ -3533,11 +3539,11 @@
       <c r="H52" s="25"/>
       <c r="I52" s="25"/>
       <c r="J52" s="25"/>
-      <c r="K52" s="27" t="s">
+      <c r="K52" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="L52" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="L52" s="17" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,10 +3551,10 @@
         <v>81</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>148</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>149</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
@@ -3558,7 +3564,7 @@
       <c r="I53" s="25"/>
       <c r="J53" s="25"/>
       <c r="K53" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L53" s="17" t="s">
         <v>140</v>
@@ -3569,10 +3575,10 @@
         <v>81</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>151</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>152</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
@@ -3594,8 +3600,8 @@
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
       <c r="J55" s="25"/>
       <c r="K55" s="22"/>
       <c r="L55" s="17"/>
@@ -3678,137 +3684,137 @@
       <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="1" width="45.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="B2" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3897,7 +3903,7 @@
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.95"/>
@@ -3905,87 +3911,87 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="43" t="n">
+        <f aca="true">NOW()</f>
+        <v>45273.6882797617</v>
+      </c>
+      <c r="D2" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="42" t="n">
-        <f aca="true">NOW()</f>
-        <v>45253.4451292648</v>
-      </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4011,1128 +4017,1128 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="1" width="45.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="B2" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
+      <c r="W16" s="40"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="40"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="40"/>
+      <c r="W24" s="40"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="40"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="40"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="40"/>
+      <c r="W28" s="40"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="39"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="39"/>
-      <c r="W9" s="39"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="39"/>
-      <c r="W12" s="39"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="39"/>
-      <c r="W15" s="39"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="39"/>
-      <c r="V16" s="39"/>
-      <c r="W16" s="39"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="39"/>
-      <c r="U18" s="39"/>
-      <c r="V18" s="39"/>
-      <c r="W18" s="39"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="39"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
-      <c r="W20" s="39"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39"/>
-      <c r="W22" s="39"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="39"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="39"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="39"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="39"/>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="39"/>
-      <c r="W27" s="39"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="39"/>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
-      <c r="V28" s="39"/>
-      <c r="W28" s="39"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="39" t="s">
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="39"/>
-      <c r="T30" s="39"/>
-      <c r="U30" s="39"/>
-      <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B31" s="39" t="s">
+      <c r="B32" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C32" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39"/>
-      <c r="V31" s="39"/>
-      <c r="W31" s="39"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>207</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
-      <c r="T32" s="39"/>
-      <c r="U32" s="39"/>
-      <c r="V32" s="39"/>
-      <c r="W32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="39"/>
-      <c r="S33" s="39"/>
-      <c r="T33" s="39"/>
-      <c r="U33" s="39"/>
-      <c r="V33" s="39"/>
-      <c r="W33" s="39"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B34" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B35" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C35, "(", ""), ")", "")), " ", "_")</f>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B36" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C36, "(", ""), ")", "")), " ", "_")</f>
         <v>injectibles</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B37" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C37, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B38" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C38, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B39" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C39, "(", ""), ")", "")), " ", "_")</f>
         <v>iud</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C40, "(", ""), ")", "")), " ", "_")</f>
         <v>condoms</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C41, "(", ""), ")", "")), " ", "_")</f>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B42" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C42, "(", ""), ")", "")), " ", "_")</f>
         <v>cycle_beads</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5143,26 +5149,26 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B45" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C45, "(", ""), ")", "")), " ", "_")</f>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" s="1" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C46, "(", ""), ")", "")), " ", "_")</f>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5172,290 +5178,290 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="C48" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+      <c r="V48" s="38"/>
+      <c r="W48" s="38"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
-      <c r="Q48" s="37"/>
-      <c r="R48" s="37"/>
-      <c r="S48" s="37"/>
-      <c r="T48" s="37"/>
-      <c r="U48" s="37"/>
-      <c r="V48" s="37"/>
-      <c r="W48" s="37"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="B49" s="38" t="s">
+      <c r="C49" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="C49" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="37"/>
-      <c r="P49" s="37"/>
-      <c r="Q49" s="37"/>
-      <c r="R49" s="37"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="37"/>
-      <c r="U49" s="37"/>
-      <c r="V49" s="37"/>
-      <c r="W49" s="37"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="38"/>
+      <c r="W49" s="38"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="38" t="s">
+      <c r="A58" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58" s="39" t="s">
         <v>237</v>
       </c>
-      <c r="B58" s="38" t="s">
+      <c r="C58" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="38" t="s">
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="39" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="B59" s="38" t="s">
+      <c r="C59" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="C59" s="38" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" s="39" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="B60" s="38" t="s">
+      <c r="C60" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="C60" s="38" t="s">
-        <v>243</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="B61" s="38" t="s">
+      <c r="A61" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" s="39" t="s">
         <v>203</v>
-      </c>
-      <c r="C61" s="38" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="C63" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="C63" s="38" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B64" s="38" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="B64" s="37" t="s">
+      <c r="C64" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="C64" s="38" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B65" s="38" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="B65" s="37" t="s">
+      <c r="C65" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="C65" s="38" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B66" s="38" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="B66" s="37" t="s">
+      <c r="C66" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="C66" s="38" t="s">
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B67" s="38" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="B67" s="37" t="s">
+      <c r="C67" s="39" t="s">
         <v>253</v>
-      </c>
-      <c r="C67" s="38" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C72" s="45" t="s">
-        <v>219</v>
+      <c r="C72" s="46" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>